<commit_message>
Add traditional data generator comparison
</commit_message>
<xml_diff>
--- a/ProjectResult_PSY.xlsx
+++ b/ProjectResult_PSY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e7af1af291dec83/DLProject/Project-Post/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{576A60DA-18A7-44BB-93AA-EACACFF68750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{576A60DA-18A7-44BB-93AA-EACACFF68750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0C22D17-E227-4360-8C8F-CE2299927961}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9A63167B-CC00-4DC1-AE3B-06E4AD6057E3}"/>
+    <workbookView xWindow="1440" yWindow="1164" windowWidth="21600" windowHeight="11340" xr2:uid="{9A63167B-CC00-4DC1-AE3B-06E4AD6057E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -625,19 +625,19 @@
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G7" s="1">
+        <v>98.7</v>
+      </c>
+      <c r="H7" s="1">
         <v>98.1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>97.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>